<commit_message>
Implemented New Design into Page Pagination System + OCR Planning
</commit_message>
<xml_diff>
--- a/Automation Data/Prototype_v2.2.xlsx
+++ b/Automation Data/Prototype_v2.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thak0\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thak0\Documents\Year3_Intership_Application\Data Entry Automation\Repos\Data-Entry-Automation\Automation Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488679F3-F31C-44B9-BA5B-24FF64608085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D711B57D-4517-4B16-B43F-0D01F55F7DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,59 +19,28 @@
     <sheet name="Linked Options" sheetId="5" r:id="rId4"/>
     <sheet name="Options" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="3">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="3">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-    <bk>
-      <rc t="1" v="1"/>
-    </bk>
-    <bk>
-      <rc t="1" v="2"/>
-    </bk>
-  </valueMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>ItemID</t>
   </si>
@@ -179,6 +148,9 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -280,80 +252,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>1</v>
-    <v>5</v>
-  </rv>
-  <rv s="0">
-    <v>2</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
-  <rel r:id="rId3"/>
-</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,7 +520,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,7 +552,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -670,11 +568,11 @@
       <c r="E2" s="2">
         <v>1.2</v>
       </c>
-      <c r="F2" s="2" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -690,11 +588,11 @@
       <c r="E3" s="2">
         <v>2.4</v>
       </c>
-      <c r="F3" s="2" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -710,8 +608,8 @@
       <c r="E4" s="2">
         <v>3.9</v>
       </c>
-      <c r="F4" s="2" t="e" vm="3">
-        <v>#VALUE!</v>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the shitty Prototype_v2.3
</commit_message>
<xml_diff>
--- a/Automation Data/Prototype_v2.2.xlsx
+++ b/Automation Data/Prototype_v2.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thak0\Documents\Year3_Intership_Application\Data Entry Automation\Repos\Data-Entry-Automation\Automation Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D711B57D-4517-4B16-B43F-0D01F55F7DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87F5FC4-BE1B-48E6-8921-19F6DD4249AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,7 +725,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,7 +857,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>